<commit_message>
Add wgs workflow README.md
</commit_message>
<xml_diff>
--- a/常用工具/常用软件统计.xlsx
+++ b/常用工具/常用软件统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wuyang/Desktop/Github_repository/BioinfoDemoLab/常用工具/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171F2C8C-1A61-744D-A17D-5C526052AF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7605B369-A00D-204B-8E5F-F19245661430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10540" yWindow="1200" windowWidth="26280" windowHeight="16740" activeTab="2" xr2:uid="{47675627-AA29-8145-A4D6-D12822050ABF}"/>
+    <workbookView xWindow="940" yWindow="2080" windowWidth="22340" windowHeight="14420" activeTab="2" xr2:uid="{47675627-AA29-8145-A4D6-D12822050ABF}"/>
   </bookViews>
   <sheets>
     <sheet name="序列比对" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="185">
   <si>
     <t>BWA</t>
   </si>
@@ -1912,69 +1912,983 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>从比对文件（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">BAM/SAM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>格式）中根据基因注释文件（如</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> GTF/GFF </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>格式）计数每个基因的读段数。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>比对后的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>sam</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>或</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>bam</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>文件。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">2. gtf </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>基因组注释文件。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>输出结果是一个包含基因名称和读段计数的文本文件，每行表示一个基因及其对应的读段数</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>支持不同计数模式，能够处理复杂基因结构，但是无法输入多个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>bam</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>文件。需要分别定量之后再合并。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>基于</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> SAM/BAM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>文件的基因表达计数</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>gene_counts.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>；</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> gene_counts.txt.summary</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.  FeatureCounts </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>生成的核心输出文件，包含了所有指定基因或特征的读段计数结果。通常是一个以制表符（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>tab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）分隔的文本文件。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>关于计数结果的统计总结信息文件（通常以</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">.summary </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>结尾）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>计算速度快，内存占用低，适用于大数据量</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> RNA-Seq </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>计数。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>建立索引，一共有两种建立索引的方式，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>基于转录本参考序列的索引构建。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>使用基因组信息增强的转录本索引构建</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>fa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>格式的参考转录本序列。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>输出一个包含</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>个索引文件的索引目录。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>快速处理大规模</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> RNA-Seq </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>数据，适合转录本水平的基因表达定量分析，但是需要有高质量的转录本参考文件。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>直接基因</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>fq</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>文件，对基因表达定量</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>salmon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>索引；</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> xxx.fq</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>索引所在的目录。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 2. fq</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>格式的测序数据。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>指定输出目录，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">quant.sf </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是保存定量结果的文本文件。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>基于比对后的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> BAM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>文件进行转录本组装和基因表达量估算。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>输出四个文件；</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>genes.fpkm_tracking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>和</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">isoforms.fpkm_tracking </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分别记录了基因水平和转录本水平的。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> skipped.gtf </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>和</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> transcripts.gtf </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分别记录了转录本组装结果和未成功</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>用于转录本组装和基因表达定量分析，适合于新转录本发现和定量。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>涉及的文件格式参考</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="14"/>
+        <color theme="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>转录本序列</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="14"/>
+        <color theme="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> cdna.fa</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gatk CombineGVCFs</t>
+  </si>
+  <si>
+    <t>gatk GenotypeGVCFs</t>
+  </si>
+  <si>
+    <t>gatk VariantFiltration</t>
+  </si>
+  <si>
+    <t>创建参考基因组的s序列字典文件（.dict），供 GATK 和其他工具使用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>genome.fa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>fa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>格式的参考基因组</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>标记 PCR 或测序过程中的重复读段，以避免在变异检测中因重复读段而产生偏差。</t>
+  </si>
+  <si>
+    <t>将多个样本的 GVCF 文件合并为一个 GVCF 文件。</t>
+  </si>
+  <si>
+    <t>BCFtools</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bcftools mpilup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bcftools call</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过堆叠比对数据生成变异候选位点的序列深度信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.xxx.bam; 2. genome.fa</t>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>比对后的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>bam</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>文件。通常是使用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">bwa; 2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>参考基因组（必须是已建立</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>faidx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>索引的）</t>
+    </r>
+  </si>
+  <si>
+    <t>xxx.vcf.gz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>从</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> BAM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>文件生成</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> pileup </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>信息，并输出用于后续变异检测的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> VCF </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>格式文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gatk CreateSequenceDictionary</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gatk MarkDuplicates</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>gatk HaplotypeCaller</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>从比对文件（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">BAM/SAM </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>格式）中根据基因注释文件（如</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> GTF/GFF </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>格式）计数每个基因的读段数。</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="1"/>
         <charset val="134"/>
       </rPr>
       <t>比对后的</t>
@@ -1986,110 +2900,27 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>sam</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>或</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t>bam</t>
     </r>
     <r>
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>文件。</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">2. gtf </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>基因组注释文件。</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>输出结果是一个包含基因名称和读段计数的文本文件，每行表示一个基因及其对应的读段数</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>支持不同计数模式，能够处理复杂基因结构，但是无法输入多个</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>bam</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>文件。需要分别定量之后再合并。</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
+        <rFont val="SimSun"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="1"/>
         <charset val="134"/>
       </rPr>
       <t>基于</t>
@@ -2101,588 +2932,42 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> SAM/BAM </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>文件的基因表达计数</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>gene_counts.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>；</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> gene_counts.txt.summary</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1.  FeatureCounts </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>生成的核心输出文件，包含了所有指定基因或特征的读段计数结果。通常是一个以制表符（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>tab</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>）分隔的文本文件。</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">2. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>关于计数结果的统计总结信息文件（通常以</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">.summary </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>结尾）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>计算速度快，内存占用低，适用于大数据量</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> RNA-Seq </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>计数。</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>建立索引，一共有两种建立索引的方式，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>基于转录本参考序列的索引构建。</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">2. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>使用基因组信息增强的转录本索引构建</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>fa</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>格式的参考转录本序列。</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>输出一个包含</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>16</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>个索引文件的索引目录。</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>快速处理大规模</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> RNA-Seq </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>数据，适合转录本水平的基因表达定量分析，但是需要有高质量的转录本参考文件。</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>直接基因</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>fq</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>文件，对基因表达定量</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>salmon</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>索引；</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> xxx.fq</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>索引所在的目录。</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 2. fq</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>格式的测序数据。</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>指定输出目录，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">quant.sf </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>是保存定量结果的文本文件。</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>基于比对后的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> BAM </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>文件进行转录本组装和基因表达量估算。</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>输出四个文件；</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>genes.fpkm_tracking</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>和</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">isoforms.fpkm_tracking </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>分别记录了基因水平和转录本水平的。</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> skipped.gtf </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>和</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> transcripts.gtf </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>分别记录了转录本组装结果和未成功</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>用于转录本组装和基因表达定量分析，适合于新转录本发现和定量。</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>涉及的文件格式参考</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="14"/>
-        <color theme="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>转录本序列</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="14"/>
-        <color theme="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> cdna.fa</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>gatk CreateSequenceDictionary</t>
-  </si>
-  <si>
-    <t>gatk MarkDuplicates</t>
-  </si>
-  <si>
-    <t>gatk CombineGVCFs</t>
-  </si>
-  <si>
-    <t>gatk GenotypeGVCFs</t>
-  </si>
-  <si>
-    <t>gatk VariantFiltration</t>
+      <t>mpilup</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>得到的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>vcf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>文件进行最终的变异调用</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bcftools filter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3026,7 +3311,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3177,15 +3462,63 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3225,6 +3558,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3232,18 +3577,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3261,58 +3594,25 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3649,16 +3949,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19" customHeight="1">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
     </row>
     <row r="2" spans="1:8" ht="34" customHeight="1" thickBot="1">
       <c r="A2" s="3" t="s">
@@ -3687,7 +3987,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="20" customHeight="1">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="80" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -3708,12 +4008,12 @@
       <c r="G3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="65" t="s">
+      <c r="H3" s="81" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20" customHeight="1">
-      <c r="A4" s="60"/>
+      <c r="A4" s="76"/>
       <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
@@ -3732,10 +4032,10 @@
       <c r="G4" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="62"/>
+      <c r="H4" s="78"/>
     </row>
     <row r="5" spans="1:8" ht="20" customHeight="1">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="75" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="11" t="s">
@@ -3756,12 +4056,12 @@
       <c r="G5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="63" t="s">
+      <c r="H5" s="79" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20" customHeight="1">
-      <c r="A6" s="60"/>
+      <c r="A6" s="76"/>
       <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
@@ -3780,10 +4080,10 @@
       <c r="G6" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="62"/>
+      <c r="H6" s="78"/>
     </row>
     <row r="7" spans="1:8" ht="20" customHeight="1">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="75" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="11" t="s">
@@ -3804,12 +4104,12 @@
       <c r="G7" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="61" t="s">
+      <c r="H7" s="77" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20" customHeight="1">
-      <c r="A8" s="60"/>
+      <c r="A8" s="76"/>
       <c r="B8" s="8" t="s">
         <v>13</v>
       </c>
@@ -3828,10 +4128,10 @@
       <c r="G8" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="62"/>
+      <c r="H8" s="78"/>
     </row>
     <row r="9" spans="1:8" ht="20" customHeight="1">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="75" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="14" t="s">
@@ -3852,12 +4152,12 @@
       <c r="G9" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="63" t="s">
+      <c r="H9" s="79" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="20" customHeight="1">
-      <c r="A10" s="60"/>
+      <c r="A10" s="76"/>
       <c r="B10" s="9" t="s">
         <v>25</v>
       </c>
@@ -3876,10 +4176,10 @@
       <c r="G10" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="62"/>
+      <c r="H10" s="78"/>
     </row>
     <row r="11" spans="1:8" ht="20" customHeight="1">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="69" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="25" t="s">
@@ -3900,12 +4200,12 @@
       <c r="G11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="H11" s="55" t="s">
+      <c r="H11" s="71" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20" customHeight="1">
-      <c r="A12" s="54"/>
+      <c r="A12" s="70"/>
       <c r="B12" s="8" t="s">
         <v>60</v>
       </c>
@@ -3922,7 +4222,7 @@
       <c r="G12" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="56"/>
+      <c r="H12" s="72"/>
     </row>
     <row r="13" spans="1:8">
       <c r="H13" s="2"/>
@@ -3987,28 +4287,28 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="52" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="52" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" style="52" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" style="52" customWidth="1"/>
-    <col min="5" max="5" width="26" style="52" customWidth="1"/>
-    <col min="6" max="6" width="22.1640625" style="52" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" style="52" customWidth="1"/>
-    <col min="8" max="8" width="41" style="52" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="50" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="50" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="50" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" style="50" customWidth="1"/>
+    <col min="5" max="5" width="26" style="50" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" style="50" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" style="50" customWidth="1"/>
+    <col min="8" max="8" width="41" style="50" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="86" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
     </row>
     <row r="2" spans="1:8" ht="34" customHeight="1" thickBot="1">
       <c r="A2" s="27" t="s">
@@ -4037,129 +4337,129 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="46" customHeight="1">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="53" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="53" t="s">
         <v>143</v>
       </c>
-      <c r="D3" s="81" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="81" t="s">
+      <c r="F3" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="F3" s="81" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" s="28" t="s">
+      <c r="H3" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="H3" s="26" t="s">
+    </row>
+    <row r="4" spans="1:8" ht="37" customHeight="1">
+      <c r="A4" s="54" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="37" customHeight="1">
-      <c r="A4" s="82" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="83" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>147</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>68</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F4" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="G4" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="H4" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="H4" s="35" t="s">
-        <v>150</v>
-      </c>
     </row>
     <row r="5" spans="1:8" ht="20" customHeight="1">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="82" t="s">
         <v>73</v>
       </c>
       <c r="B5" s="34" t="s">
         <v>74</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D5" s="34" t="s">
         <v>75</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F5" s="35" t="s">
         <v>76</v>
       </c>
       <c r="G5" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="H5" s="84" t="s">
         <v>153</v>
       </c>
-      <c r="H5" s="70" t="s">
-        <v>154</v>
-      </c>
     </row>
     <row r="6" spans="1:8" ht="23" customHeight="1">
-      <c r="A6" s="69"/>
+      <c r="A6" s="83"/>
       <c r="B6" s="33" t="s">
         <v>77</v>
       </c>
       <c r="C6" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="E6" s="33" t="s">
         <v>156</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>157</v>
       </c>
       <c r="F6" s="36" t="s">
         <v>78</v>
       </c>
       <c r="G6" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="H6" s="85"/>
+    </row>
+    <row r="7" spans="1:8" ht="40" customHeight="1">
+      <c r="A7" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="57" t="s">
         <v>158</v>
       </c>
-      <c r="H6" s="71"/>
-    </row>
-    <row r="7" spans="1:8" ht="40" customHeight="1">
-      <c r="A7" s="84" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="85" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="85" t="s">
+      <c r="D7" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="58" t="s">
+        <v>143</v>
+      </c>
+      <c r="F7" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="57" t="s">
         <v>159</v>
       </c>
-      <c r="D7" s="86" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="86" t="s">
-        <v>144</v>
-      </c>
-      <c r="F7" s="85" t="s">
-        <v>82</v>
-      </c>
-      <c r="G7" s="85" t="s">
+      <c r="H7" s="57" t="s">
         <v>160</v>
-      </c>
-      <c r="H7" s="85" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18" customHeight="1">
@@ -4173,24 +4473,24 @@
       <c r="H8" s="28"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="87" t="s">
+      <c r="A10" s="59" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="60" t="s">
         <v>162</v>
       </c>
-      <c r="B10" s="88" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="88" t="s">
-        <v>163</v>
-      </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="87"/>
-      <c r="B11" s="89"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="89"/>
-      <c r="E11" s="89"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
+      <c r="A11" s="59"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
     </row>
     <row r="12" spans="1:8">
       <c r="H12" s="28"/>
@@ -4216,32 +4516,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EF59A2-F1BF-1F4B-9B11-0F651E048B19}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="18.33203125" style="28" customWidth="1"/>
-    <col min="2" max="2" width="22.5" style="28" customWidth="1"/>
-    <col min="3" max="7" width="14.83203125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" style="28" customWidth="1"/>
+    <col min="5" max="7" width="14.83203125" style="28" customWidth="1"/>
     <col min="8" max="8" width="39.1640625" style="28" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19" customHeight="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="86" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
     </row>
     <row r="2" spans="1:8" ht="25" customHeight="1" thickBot="1">
       <c r="A2" s="27" t="s">
@@ -4270,7 +4572,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="31" customHeight="1">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="92" t="s">
         <v>83</v>
       </c>
       <c r="B3" s="31" t="s">
@@ -4291,12 +4593,12 @@
       <c r="G3" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="H3" s="67" t="s">
+      <c r="H3" s="87" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="31" customHeight="1">
-      <c r="A4" s="76"/>
+      <c r="A4" s="92"/>
       <c r="B4" s="28" t="s">
         <v>104</v>
       </c>
@@ -4315,10 +4617,10 @@
       <c r="G4" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="H4" s="67"/>
+      <c r="H4" s="87"/>
     </row>
     <row r="5" spans="1:8" ht="31" customHeight="1">
-      <c r="A5" s="76"/>
+      <c r="A5" s="92"/>
       <c r="B5" s="38" t="s">
         <v>105</v>
       </c>
@@ -4337,10 +4639,10 @@
       <c r="G5" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="H5" s="67"/>
+      <c r="H5" s="87"/>
     </row>
     <row r="6" spans="1:8" ht="27" customHeight="1">
-      <c r="A6" s="77"/>
+      <c r="A6" s="93"/>
       <c r="B6" s="49" t="s">
         <v>106</v>
       </c>
@@ -4359,16 +4661,16 @@
       <c r="G6" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="H6" s="71"/>
+      <c r="H6" s="85"/>
     </row>
     <row r="7" spans="1:8" ht="45" customHeight="1">
-      <c r="A7" s="95" t="s">
+      <c r="A7" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="64" t="s">
         <v>134</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="65" t="s">
         <v>135</v>
       </c>
       <c r="D7" s="34" t="s">
@@ -4388,132 +4690,180 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="24" customHeight="1">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="82" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="94" t="s">
-        <v>164</v>
-      </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
+      <c r="B8" s="62" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>168</v>
+      </c>
       <c r="F8" s="35"/>
       <c r="G8" s="35"/>
-      <c r="H8" s="70"/>
+      <c r="H8" s="84"/>
     </row>
     <row r="9" spans="1:8" ht="24" customHeight="1">
-      <c r="A9" s="90"/>
-      <c r="B9" s="94" t="s">
+      <c r="A9" s="94"/>
+      <c r="B9" s="62" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" t="s">
+        <v>169</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>182</v>
+      </c>
+      <c r="H9" s="87"/>
+    </row>
+    <row r="10" spans="1:8" ht="24" customHeight="1">
+      <c r="A10" s="94"/>
+      <c r="B10" s="62" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="H10" s="87"/>
+    </row>
+    <row r="11" spans="1:8" ht="24" customHeight="1">
+      <c r="A11" s="94"/>
+      <c r="B11" s="62" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" t="s">
+        <v>170</v>
+      </c>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="H11" s="87"/>
+    </row>
+    <row r="12" spans="1:8" ht="24" customHeight="1">
+      <c r="A12" s="94"/>
+      <c r="B12" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="H12" s="87"/>
+    </row>
+    <row r="13" spans="1:8" ht="23" customHeight="1">
+      <c r="A13" s="83"/>
+      <c r="B13" s="62" t="s">
         <v>165</v>
-      </c>
-      <c r="C9" s="91"/>
-      <c r="D9" s="91"/>
-      <c r="E9" s="91"/>
-      <c r="F9" s="92"/>
-      <c r="G9" s="92"/>
-      <c r="H9" s="93"/>
-    </row>
-    <row r="10" spans="1:8" ht="24" customHeight="1">
-      <c r="A10" s="90"/>
-      <c r="B10" s="94" t="s">
-        <v>142</v>
-      </c>
-      <c r="C10" s="91"/>
-      <c r="D10" s="91"/>
-      <c r="E10" s="91"/>
-      <c r="F10" s="92"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="93"/>
-    </row>
-    <row r="11" spans="1:8" ht="24" customHeight="1">
-      <c r="A11" s="90"/>
-      <c r="B11" s="94" t="s">
-        <v>166</v>
-      </c>
-      <c r="C11" s="91"/>
-      <c r="D11" s="91"/>
-      <c r="E11" s="91"/>
-      <c r="F11" s="92"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="93"/>
-    </row>
-    <row r="12" spans="1:8" ht="24" customHeight="1">
-      <c r="A12" s="90"/>
-      <c r="B12" s="94" t="s">
-        <v>167</v>
-      </c>
-      <c r="C12" s="91"/>
-      <c r="D12" s="91"/>
-      <c r="E12" s="91"/>
-      <c r="F12" s="92"/>
-      <c r="G12" s="92"/>
-      <c r="H12" s="93"/>
-    </row>
-    <row r="13" spans="1:8" ht="23" customHeight="1">
-      <c r="A13" s="69"/>
-      <c r="B13" s="94" t="s">
-        <v>168</v>
       </c>
       <c r="C13" s="33"/>
       <c r="D13" s="33"/>
       <c r="E13" s="33"/>
       <c r="G13" s="36"/>
-      <c r="H13" s="71"/>
+      <c r="H13" s="85"/>
     </row>
     <row r="14" spans="1:8" ht="20" customHeight="1">
-      <c r="A14" s="68"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="70"/>
+      <c r="A14" s="82" t="s">
+        <v>171</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" s="66" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="G14" s="67" t="s">
+        <v>178</v>
+      </c>
+      <c r="H14" s="84"/>
     </row>
     <row r="15" spans="1:8" ht="20" customHeight="1">
-      <c r="A15" s="69"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="71"/>
+      <c r="A15" s="94"/>
+      <c r="B15" s="96" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" s="100" t="s">
+        <v>183</v>
+      </c>
+      <c r="D15" s="96" t="s">
+        <v>119</v>
+      </c>
+      <c r="E15" s="96"/>
+      <c r="F15" s="97"/>
+      <c r="G15" s="98"/>
+      <c r="H15" s="99"/>
     </row>
     <row r="16" spans="1:8" ht="20" customHeight="1">
-      <c r="A16" s="72"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="H16" s="74"/>
+      <c r="A16" s="94"/>
+      <c r="B16" s="96" t="s">
+        <v>184</v>
+      </c>
+      <c r="C16" s="100"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="97"/>
+      <c r="G16" s="98"/>
+      <c r="H16" s="99"/>
     </row>
     <row r="17" spans="1:8" ht="20" customHeight="1">
-      <c r="A17" s="73"/>
+      <c r="A17" s="83"/>
       <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
+      <c r="C17" s="68"/>
       <c r="D17" s="33"/>
       <c r="E17" s="33"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="75"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="29" t="s">
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="85"/>
+    </row>
+    <row r="18" spans="1:8" ht="20" customHeight="1">
+      <c r="A18" s="88"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="H18" s="90"/>
+    </row>
+    <row r="19" spans="1:8" ht="20" customHeight="1">
+      <c r="A19" s="89"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="91"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="29" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="79" t="s">
+    <row r="25" spans="1:8">
+      <c r="A25" s="51" t="s">
         <v>140</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="H18:H19"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="H3:H6"/>
@@ -4522,9 +4872,9 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1" xr:uid="{E749A47B-FC7F-3F42-9E3E-E5E7DC46933C}"/>
+    <hyperlink ref="A23" r:id="rId1" xr:uid="{E749A47B-FC7F-3F42-9E3E-E5E7DC46933C}"/>
     <hyperlink ref="A3:A6" r:id="rId2" display="LoFreq" xr:uid="{7BBE7D8C-97E2-BA49-9BBB-E033AF299A97}"/>
-    <hyperlink ref="A23" r:id="rId3" xr:uid="{1F2C2774-9A84-964E-9ECA-3BB0767CC27B}"/>
+    <hyperlink ref="A25" r:id="rId3" xr:uid="{1F2C2774-9A84-964E-9ECA-3BB0767CC27B}"/>
     <hyperlink ref="A7" r:id="rId4" xr:uid="{3F7D9DB8-7C53-FD4D-B9E6-E9A60C3F7082}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4548,16 +4898,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="44" customHeight="1">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="95" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
     </row>
     <row r="2" spans="1:8" ht="34" customHeight="1" thickBot="1">
       <c r="A2" s="27" t="s">

</xml_diff>